<commit_message>
Added columns for path parameters
</commit_message>
<xml_diff>
--- a/test/endpoints/templates/delete-data-tests.xlsx
+++ b/test/endpoints/templates/delete-data-tests.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -411,6 +411,8 @@
     <col min="6" max="6" customWidth="1" width="15"/>
     <col min="7" max="7" customWidth="1" width="15"/>
     <col min="8" max="8" customWidth="1" width="15"/>
+    <col min="9" max="9" customWidth="1" width="20"/>
+    <col min="10" max="10" customWidth="1" width="20"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -438,6 +440,12 @@
       <c r="H1" t="str">
         <v>tags</v>
       </c>
+      <c r="I1" t="str">
+        <v>param:type</v>
+      </c>
+      <c r="J1" t="str">
+        <v>param:uuid</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -464,17 +472,55 @@
       <c r="H2" t="str">
         <v>delete-data,functional</v>
       </c>
+      <c r="I2" t="str">
+        <v>work</v>
+      </c>
+      <c r="J2" t="str">
+        <v>12345678-1234-1234-1234-123456789abc</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>delete-data - Missing Required Param</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Test DELETE /data/:type/:uuid with missing required parameters</v>
+      </c>
+      <c r="C3" t="str">
+        <v>true</v>
+      </c>
+      <c r="D3">
+        <v>400</v>
+      </c>
+      <c r="E3">
+        <v>10000</v>
+      </c>
+      <c r="F3">
+        <v>2000</v>
+      </c>
+      <c r="G3">
+        <v>500</v>
+      </c>
+      <c r="H3" t="str">
+        <v>delete-data,validation</v>
+      </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
+      <c r="J3" t="str">
+        <v>12345678-1234-1234-1234-123456789abc</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -594,37 +640,63 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v/>
+        <v>Parameter Descriptions:</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Endpoint-Specific Notes:</v>
+        <v>param:type</v>
+      </c>
+      <c r="B18" t="str">
+        <v>type parameter (string) (REQUIRED - highlighted in yellow)</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>• Method: DELETE</v>
+        <v>param:uuid</v>
+      </c>
+      <c r="B19" t="str">
+        <v>uuid parameter (string) (REQUIRED - highlighted in yellow)</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>• Path: /data/:type/:uuid</v>
+        <v/>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>• Description: Delete a document by type and UUID</v>
+        <v>Endpoint-Specific Notes:</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
+        <v>• Method: DELETE</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>• Path: /data/:type/:uuid</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>• Description: Delete a document by type and UUID</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>• Required parameters: type, uuid</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
         <v>• Document operations may require different parameters based on the operation type</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B22"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B26"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>